<commit_message>
updated meeting minutes and added work plan
</commit_message>
<xml_diff>
--- a/Project Management/Meeting_Minutes/Log of Meetings.xlsx
+++ b/Project Management/Meeting_Minutes/Log of Meetings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Molly Meadows\OneDrive - University of Idaho\Documents\2023-2024\Capstone Project\26-Physical-Rehabilitation\Meeting_Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Molly Meadows\OneDrive - University of Idaho\Documents\2023-2024\Capstone Project\26-Physical-Rehabilitation\Project Management\Meeting_Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B112143D-FCE8-43B4-9D68-9695AE8A5C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CECDCE9-937A-4BDB-ABA4-A042AEE79756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11976" yWindow="0" windowWidth="8304" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>35 minutes</t>
+  </si>
+  <si>
+    <t>4:15pm</t>
+  </si>
+  <si>
+    <t>3:45pm</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Progress update and discussion of libraries for skeletal extraction. Set up a meeting with client</t>
+  </si>
+  <si>
+    <t>3:00pm</t>
+  </si>
+  <si>
+    <t>3:30pm</t>
+  </si>
+  <si>
+    <t>Client meeting to discuss progress. Was given access to a layout for our project and videos for analysis. Switched first exercise to deep squat</t>
   </si>
 </sst>
 </file>
@@ -125,10 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,6 +514,40 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45196</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update meeting minutes and log
</commit_message>
<xml_diff>
--- a/Project Management/Meeting_Minutes/Log of Meetings.xlsx
+++ b/Project Management/Meeting_Minutes/Log of Meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Molly Meadows\OneDrive - University of Idaho\Documents\2023-2024\Capstone Project\26-Physical-Rehabilitation\Project Management\Meeting_Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CECDCE9-937A-4BDB-ABA4-A042AEE79756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF410A20-362C-468F-8170-42F6F45A42AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11976" yWindow="0" windowWidth="8304" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Client meeting to discuss progress. Was given access to a layout for our project and videos for analysis. Switched first exercise to deep squat</t>
+  </si>
+  <si>
+    <t>10:00am</t>
+  </si>
+  <si>
+    <t>10:45pm</t>
+  </si>
+  <si>
+    <t>45 minutes</t>
+  </si>
+  <si>
+    <t>Update and design concept review discussion</t>
   </si>
 </sst>
 </file>
@@ -431,19 +443,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="117.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -548,6 +560,23 @@
         <v>22</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>